<commit_message>
commiting files after week logic sucsess
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Shared ParentalPay201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Shared ParentalPay201718.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="18" firstSheet="17" windowHeight="5400" windowWidth="15168" xWindow="396" yWindow="36"/>
+    <workbookView activeTab="5" firstSheet="3" windowHeight="5400" windowWidth="15168" xWindow="396" yWindow="36"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="210">
   <si>
     <t>TC</t>
   </si>
@@ -458,9 +458,6 @@
   </si>
   <si>
     <t>DO NOT TOUCH AUTOMATION ShPP 101</t>
-  </si>
-  <si>
-    <t>Week-11</t>
   </si>
   <si>
     <t>DO NOT TOUCH ShPP GROSS PAYMENTS</t>
@@ -1188,10 +1185,10 @@
     </row>
     <row ht="30" r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
@@ -1202,10 +1199,10 @@
     </row>
     <row ht="15" r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -1216,10 +1213,10 @@
     </row>
     <row ht="30" r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -1230,10 +1227,10 @@
     </row>
     <row ht="15" r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
@@ -1244,10 +1241,10 @@
     </row>
     <row ht="30" r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
@@ -1258,10 +1255,10 @@
     </row>
     <row ht="15" r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
@@ -1272,10 +1269,10 @@
     </row>
     <row ht="30" r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
@@ -1286,10 +1283,10 @@
     </row>
     <row ht="15" r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
@@ -1300,10 +1297,10 @@
     </row>
     <row ht="30" r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
@@ -1314,10 +1311,10 @@
     </row>
     <row ht="15" r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
@@ -1328,10 +1325,10 @@
     </row>
     <row ht="30" r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>4</v>
@@ -1342,10 +1339,10 @@
     </row>
     <row ht="15" r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>4</v>
@@ -1356,10 +1353,10 @@
     </row>
     <row ht="30" r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>4</v>
@@ -1370,10 +1367,10 @@
     </row>
     <row ht="15" r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
@@ -1384,10 +1381,10 @@
     </row>
     <row ht="30" r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
@@ -1398,10 +1395,10 @@
     </row>
     <row ht="15" r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1412,10 +1409,10 @@
     </row>
     <row ht="30" r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>4</v>
@@ -1426,10 +1423,10 @@
     </row>
     <row ht="15" r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>4</v>
@@ -1457,7 +1454,7 @@
         <v>131</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
@@ -1468,10 +1465,10 @@
     </row>
     <row ht="30" r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>4</v>
@@ -1482,10 +1479,10 @@
     </row>
     <row ht="15" r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>4</v>
@@ -1496,10 +1493,10 @@
     </row>
     <row ht="30" r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>4</v>
@@ -1510,10 +1507,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>4</v>
@@ -1524,10 +1521,10 @@
     </row>
     <row ht="28.8" r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
@@ -1538,10 +1535,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>4</v>
@@ -1606,7 +1603,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -1620,37 +1617,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -1716,7 +1713,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -1730,37 +1727,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -1826,7 +1823,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -1840,37 +1837,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -1936,7 +1933,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -1950,37 +1947,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -2046,7 +2043,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2060,37 +2057,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -2168,25 +2165,25 @@
         <v>141</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>111</v>
@@ -2253,7 +2250,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2267,35 +2264,35 @@
     </row>
     <row customFormat="1" customHeight="1" ht="62.4" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -2361,7 +2358,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2375,37 +2372,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -2471,7 +2468,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2485,37 +2482,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -2533,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -2581,7 +2578,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2595,37 +2592,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>155</v>
-      </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -2659,10 +2656,10 @@
         <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2679,7 +2676,7 @@
         <v>141</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>111</v>
@@ -3220,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3271,7 +3268,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -3285,37 +3282,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>143</v>
-      </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -3382,7 +3379,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -3396,37 +3393,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -3493,7 +3490,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -3507,37 +3504,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
@@ -3604,7 +3601,7 @@
         <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -3618,37 +3615,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>122</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>

</xml_diff>